<commit_message>
commit branch for build framework
</commit_message>
<xml_diff>
--- a/doc/assets/excel/库表设计.xlsx
+++ b/doc/assets/excel/库表设计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuzhengwei/itstack/git/KnowledgePlanet/Lottery/doc/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A9A07C-29E0-3B4C-84B2-9CAE16FFB711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358CA908-F6B0-FE44-AF43-EC490F5895DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{5B78EA90-A27C-8449-8C80-8B90733ED9B9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>活动表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,22 @@
   </si>
   <si>
     <t>updateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activityName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activityDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ADDC7C-5C2B-A64C-887C-A95B3C2B04B8}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C3" sqref="C3:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -581,86 +597,103 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>